<commit_message>
rename unit tests for easier monitoring and accountability
</commit_message>
<xml_diff>
--- a/Project Timeline.xlsx
+++ b/Project Timeline.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB9453A-0DF0-4333-A5D7-F75F62A4DA1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48CFA508-AAAE-4CC0-AF09-764648E03DA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -210,9 +210,6 @@
     <t>QA Test Cases</t>
   </si>
   <si>
-    <t>Deployment Of Game</t>
-  </si>
-  <si>
     <t>Assignment Report</t>
   </si>
   <si>
@@ -220,6 +217,9 @@
   </si>
   <si>
     <t>Everyone</t>
+  </si>
+  <si>
+    <t>Continous Deployment Of Game</t>
   </si>
 </sst>
 </file>
@@ -811,6 +811,13 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -823,13 +830,6 @@
     <xf numFmtId="166" fontId="9" fillId="0" borderId="3" xfId="9">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
@@ -1343,8 +1343,8 @@
   <dimension ref="A1:BL30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
+      <pane ySplit="6" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AT23" sqref="AT23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1366,7 +1366,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="53" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
@@ -1389,119 +1389,119 @@
         <v>15</v>
       </c>
       <c r="B3" s="55"/>
-      <c r="C3" s="80" t="s">
+      <c r="C3" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="81"/>
-      <c r="E3" s="79">
+      <c r="D3" s="77"/>
+      <c r="E3" s="82">
         <f>DATE(2020,1,20)</f>
         <v>43850</v>
       </c>
-      <c r="F3" s="79"/>
+      <c r="F3" s="82"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="49" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="75"/>
-      <c r="C4" s="80" t="s">
+      <c r="C4" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="81"/>
+      <c r="D4" s="77"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="76">
+      <c r="I4" s="79">
         <f>I5</f>
         <v>43850</v>
       </c>
-      <c r="J4" s="77"/>
-      <c r="K4" s="77"/>
-      <c r="L4" s="77"/>
-      <c r="M4" s="77"/>
-      <c r="N4" s="77"/>
-      <c r="O4" s="78"/>
-      <c r="P4" s="76">
+      <c r="J4" s="80"/>
+      <c r="K4" s="80"/>
+      <c r="L4" s="80"/>
+      <c r="M4" s="80"/>
+      <c r="N4" s="80"/>
+      <c r="O4" s="81"/>
+      <c r="P4" s="79">
         <f>P5</f>
         <v>43857</v>
       </c>
-      <c r="Q4" s="77"/>
-      <c r="R4" s="77"/>
-      <c r="S4" s="77"/>
-      <c r="T4" s="77"/>
-      <c r="U4" s="77"/>
-      <c r="V4" s="78"/>
-      <c r="W4" s="76">
+      <c r="Q4" s="80"/>
+      <c r="R4" s="80"/>
+      <c r="S4" s="80"/>
+      <c r="T4" s="80"/>
+      <c r="U4" s="80"/>
+      <c r="V4" s="81"/>
+      <c r="W4" s="79">
         <f>W5</f>
         <v>43864</v>
       </c>
-      <c r="X4" s="77"/>
-      <c r="Y4" s="77"/>
-      <c r="Z4" s="77"/>
-      <c r="AA4" s="77"/>
-      <c r="AB4" s="77"/>
-      <c r="AC4" s="78"/>
-      <c r="AD4" s="76">
+      <c r="X4" s="80"/>
+      <c r="Y4" s="80"/>
+      <c r="Z4" s="80"/>
+      <c r="AA4" s="80"/>
+      <c r="AB4" s="80"/>
+      <c r="AC4" s="81"/>
+      <c r="AD4" s="79">
         <f>AD5</f>
         <v>43871</v>
       </c>
-      <c r="AE4" s="77"/>
-      <c r="AF4" s="77"/>
-      <c r="AG4" s="77"/>
-      <c r="AH4" s="77"/>
-      <c r="AI4" s="77"/>
-      <c r="AJ4" s="78"/>
-      <c r="AK4" s="76">
+      <c r="AE4" s="80"/>
+      <c r="AF4" s="80"/>
+      <c r="AG4" s="80"/>
+      <c r="AH4" s="80"/>
+      <c r="AI4" s="80"/>
+      <c r="AJ4" s="81"/>
+      <c r="AK4" s="79">
         <f>AK5</f>
         <v>43878</v>
       </c>
-      <c r="AL4" s="77"/>
-      <c r="AM4" s="77"/>
-      <c r="AN4" s="77"/>
-      <c r="AO4" s="77"/>
-      <c r="AP4" s="77"/>
-      <c r="AQ4" s="78"/>
-      <c r="AR4" s="76">
+      <c r="AL4" s="80"/>
+      <c r="AM4" s="80"/>
+      <c r="AN4" s="80"/>
+      <c r="AO4" s="80"/>
+      <c r="AP4" s="80"/>
+      <c r="AQ4" s="81"/>
+      <c r="AR4" s="79">
         <f>AR5</f>
         <v>43885</v>
       </c>
-      <c r="AS4" s="77"/>
-      <c r="AT4" s="77"/>
-      <c r="AU4" s="77"/>
-      <c r="AV4" s="77"/>
-      <c r="AW4" s="77"/>
-      <c r="AX4" s="78"/>
-      <c r="AY4" s="76">
+      <c r="AS4" s="80"/>
+      <c r="AT4" s="80"/>
+      <c r="AU4" s="80"/>
+      <c r="AV4" s="80"/>
+      <c r="AW4" s="80"/>
+      <c r="AX4" s="81"/>
+      <c r="AY4" s="79">
         <f>AY5</f>
         <v>43892</v>
       </c>
-      <c r="AZ4" s="77"/>
-      <c r="BA4" s="77"/>
-      <c r="BB4" s="77"/>
-      <c r="BC4" s="77"/>
-      <c r="BD4" s="77"/>
-      <c r="BE4" s="78"/>
-      <c r="BF4" s="76">
+      <c r="AZ4" s="80"/>
+      <c r="BA4" s="80"/>
+      <c r="BB4" s="80"/>
+      <c r="BC4" s="80"/>
+      <c r="BD4" s="80"/>
+      <c r="BE4" s="81"/>
+      <c r="BF4" s="79">
         <f>BF5</f>
         <v>43899</v>
       </c>
-      <c r="BG4" s="77"/>
-      <c r="BH4" s="77"/>
-      <c r="BI4" s="77"/>
-      <c r="BJ4" s="77"/>
-      <c r="BK4" s="77"/>
-      <c r="BL4" s="78"/>
+      <c r="BG4" s="80"/>
+      <c r="BH4" s="80"/>
+      <c r="BI4" s="80"/>
+      <c r="BJ4" s="80"/>
+      <c r="BK4" s="80"/>
+      <c r="BL4" s="81"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="82"/>
-      <c r="C5" s="82"/>
-      <c r="D5" s="82"/>
-      <c r="E5" s="82"/>
-      <c r="F5" s="82"/>
-      <c r="G5" s="82"/>
+      <c r="B5" s="78"/>
+      <c r="C5" s="78"/>
+      <c r="D5" s="78"/>
+      <c r="E5" s="78"/>
+      <c r="F5" s="78"/>
+      <c r="G5" s="78"/>
       <c r="I5" s="11">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>43850</v>
@@ -2609,12 +2609,12 @@
         <v>1</v>
       </c>
       <c r="E15" s="57">
-        <f>DATE(2020,1,31)</f>
-        <v>43861</v>
+        <f>DATE(2020,2,1)</f>
+        <v>43862</v>
       </c>
       <c r="F15" s="57">
         <f>E15</f>
-        <v>43861</v>
+        <v>43862</v>
       </c>
       <c r="G15" s="17"/>
       <c r="H15" s="17">
@@ -2691,11 +2691,11 @@
       </c>
       <c r="E16" s="57">
         <f>E15</f>
-        <v>43861</v>
+        <v>43862</v>
       </c>
       <c r="F16" s="57">
         <f>E16</f>
-        <v>43861</v>
+        <v>43862</v>
       </c>
       <c r="G16" s="17"/>
       <c r="H16" s="17">
@@ -2771,12 +2771,12 @@
         <v>1</v>
       </c>
       <c r="E17" s="57">
-        <f>F16</f>
-        <v>43861</v>
+        <f>F16+1</f>
+        <v>43863</v>
       </c>
       <c r="F17" s="57">
         <f>E17+1</f>
-        <v>43862</v>
+        <v>43864</v>
       </c>
       <c r="G17" s="17"/>
       <c r="H17" s="17">
@@ -2849,20 +2849,20 @@
         <v>37</v>
       </c>
       <c r="D18" s="27">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E18" s="57">
-        <f>E17</f>
-        <v>43861</v>
+        <f>F17</f>
+        <v>43864</v>
       </c>
       <c r="F18" s="57">
-        <f>E18+3</f>
-        <v>43864</v>
+        <f>E18+1</f>
+        <v>43865</v>
       </c>
       <c r="G18" s="17"/>
       <c r="H18" s="17">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I18" s="44"/>
       <c r="J18" s="44"/>
@@ -2930,20 +2930,20 @@
         <v>37</v>
       </c>
       <c r="D19" s="27">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E19" s="57">
-        <f>E18</f>
-        <v>43861</v>
+        <f>F18</f>
+        <v>43865</v>
       </c>
       <c r="F19" s="57">
-        <f>E19+3</f>
-        <v>43864</v>
+        <f>E19+1</f>
+        <v>43866</v>
       </c>
       <c r="G19" s="17"/>
       <c r="H19" s="17">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I19" s="44"/>
       <c r="J19" s="44"/>
@@ -3159,7 +3159,7 @@
     <row r="22" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="48"/>
       <c r="B22" s="72" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C22" s="66" t="s">
         <v>34</v>
@@ -3172,13 +3172,13 @@
         <v>43863</v>
       </c>
       <c r="F22" s="58">
-        <f>E22+1</f>
-        <v>43864</v>
+        <f>E22+4</f>
+        <v>43867</v>
       </c>
       <c r="G22" s="17"/>
       <c r="H22" s="17">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I22" s="44"/>
       <c r="J22" s="44"/>
@@ -3319,20 +3319,20 @@
         <v>37</v>
       </c>
       <c r="D24" s="37">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E24" s="59">
-        <f>DATE(2020,1,29)</f>
-        <v>43859</v>
+        <f>DATE(2020,2,1)</f>
+        <v>43862</v>
       </c>
       <c r="F24" s="59">
-        <f>DATE(2020,1,31)</f>
-        <v>43861</v>
+        <f>DATE(2020,2,5)</f>
+        <v>43866</v>
       </c>
       <c r="G24" s="17"/>
       <c r="H24" s="17">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I24" s="44"/>
       <c r="J24" s="44"/>
@@ -3394,10 +3394,10 @@
     <row r="25" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="48"/>
       <c r="B25" s="73" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C25" s="68" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D25" s="37">
         <v>0.1</v>
@@ -3628,11 +3628,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
@@ -3640,6 +3635,11 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D27">
     <cfRule type="dataBar" priority="14">

</xml_diff>